<commit_message>
Trying to figure out how to interpolate...
</commit_message>
<xml_diff>
--- a/handlocations/importfile_lokaties_PT.xlsx
+++ b/handlocations/importfile_lokaties_PT.xlsx
@@ -13,10 +13,6 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -360,199 +356,179 @@
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:14">
       <c r="A1">
         <v>0.51</v>
       </c>
       <c r="B1">
+        <v>0.52</v>
+      </c>
+      <c r="C1">
+        <v>0.4</v>
+      </c>
+      <c r="D1">
+        <v>0.64</v>
+      </c>
+      <c r="E1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="F1">
+        <v>0.6</v>
+      </c>
+      <c r="G1">
+        <v>0.85</v>
+      </c>
+      <c r="H1">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I1">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="J1">
+        <v>0.52</v>
+      </c>
+      <c r="K1">
+        <v>0.72</v>
+      </c>
+      <c r="L1">
+        <v>0.77</v>
+      </c>
+      <c r="M1">
+        <v>1.28</v>
+      </c>
+      <c r="N1">
+        <v>1.1399999999999999</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
         <v>0.51</v>
-      </c>
-      <c r="C1">
-        <v>0.37</v>
-      </c>
-      <c r="D1">
-        <v>0.34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>0.52</v>
       </c>
       <c r="B2">
         <v>0.53</v>
       </c>
       <c r="C2">
+        <v>0.72</v>
+      </c>
+      <c r="D2">
+        <v>0.24</v>
+      </c>
+      <c r="E2">
+        <v>0.44</v>
+      </c>
+      <c r="F2">
+        <v>0.69</v>
+      </c>
+      <c r="G2">
+        <v>0.76</v>
+      </c>
+      <c r="H2">
+        <v>0.44</v>
+      </c>
+      <c r="I2">
+        <v>0.31</v>
+      </c>
+      <c r="J2">
+        <v>0.44</v>
+      </c>
+      <c r="K2">
+        <v>0.85</v>
+      </c>
+      <c r="L2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M2">
+        <v>0.93</v>
+      </c>
+      <c r="N2">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>0.37</v>
+      </c>
+      <c r="B3">
         <v>0.3</v>
-      </c>
-      <c r="D2">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3">
-        <v>0.4</v>
-      </c>
-      <c r="B3">
-        <v>0.72</v>
       </c>
       <c r="C3">
         <v>0.36</v>
       </c>
       <c r="D3">
+        <v>0.27</v>
+      </c>
+      <c r="E3">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F3">
         <v>0.34</v>
       </c>
+      <c r="G3">
+        <v>0.35</v>
+      </c>
+      <c r="H3">
+        <v>0.23</v>
+      </c>
+      <c r="I3">
+        <v>0.16</v>
+      </c>
+      <c r="J3">
+        <v>0.32</v>
+      </c>
+      <c r="K3">
+        <v>0.37</v>
+      </c>
+      <c r="L3">
+        <v>0.67</v>
+      </c>
+      <c r="M3">
+        <v>0.38</v>
+      </c>
+      <c r="N3">
+        <v>0.95</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:14">
       <c r="A4">
-        <v>0.64</v>
+        <v>0.34</v>
       </c>
       <c r="B4">
-        <v>0.24</v>
+        <v>0.15</v>
       </c>
       <c r="C4">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="D4">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="B5">
-        <v>0.44</v>
-      </c>
-      <c r="C5">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="D5">
+      <c r="E4">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>0.6</v>
-      </c>
-      <c r="B6">
-        <v>0.69</v>
-      </c>
-      <c r="C6">
-        <v>0.34</v>
-      </c>
-      <c r="D6">
+      <c r="F4">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>0.85</v>
-      </c>
-      <c r="B7">
-        <v>0.76</v>
-      </c>
-      <c r="C7">
+      <c r="G4">
+        <v>0.37</v>
+      </c>
+      <c r="H4">
+        <v>0.26</v>
+      </c>
+      <c r="I4">
+        <v>0.32</v>
+      </c>
+      <c r="J4">
+        <v>0.38</v>
+      </c>
+      <c r="K4">
         <v>0.35</v>
       </c>
-      <c r="D7">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>0.56000000000000005</v>
-      </c>
-      <c r="B8">
-        <v>0.44</v>
-      </c>
-      <c r="C8">
-        <v>0.23</v>
-      </c>
-      <c r="D8">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>0.57999999999999996</v>
-      </c>
-      <c r="B9">
-        <v>0.31</v>
-      </c>
-      <c r="C9">
-        <v>0.16</v>
-      </c>
-      <c r="D9">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>0.52</v>
-      </c>
-      <c r="B10">
-        <v>0.44</v>
-      </c>
-      <c r="C10">
-        <v>0.32</v>
-      </c>
-      <c r="D10">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>0.72</v>
-      </c>
-      <c r="B11">
-        <v>0.85</v>
-      </c>
-      <c r="C11">
-        <v>0.37</v>
-      </c>
-      <c r="D11">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12">
-        <v>0.77</v>
-      </c>
-      <c r="B12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C12">
-        <v>0.67</v>
-      </c>
-      <c r="D12">
+      <c r="L4">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>1.28</v>
-      </c>
-      <c r="B13">
-        <v>0.93</v>
-      </c>
-      <c r="C13">
-        <v>0.38</v>
-      </c>
-      <c r="D13">
+      <c r="M4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>1.1399999999999999</v>
-      </c>
-      <c r="B14">
-        <v>1.25</v>
-      </c>
-      <c r="C14">
-        <v>0.95</v>
-      </c>
-      <c r="D14">
+      <c r="N4">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
handlocation files op git gezet
</commit_message>
<xml_diff>
--- a/handlocations/importfile_lokaties_PT.xlsx
+++ b/handlocations/importfile_lokaties_PT.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-5325" yWindow="975" windowWidth="14445" windowHeight="12075"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="23955" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,35 @@
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>daniel_l</t>
+  </si>
+  <si>
+    <t>daniel_r</t>
+  </si>
+  <si>
+    <t>paul_l</t>
+  </si>
+  <si>
+    <t>paul_r</t>
+  </si>
+  <si>
+    <t>rienco_l</t>
+  </si>
+  <si>
+    <t>rienco_r</t>
+  </si>
+  <si>
+    <t>thijs_l</t>
+  </si>
+  <si>
+    <t>thijs_r</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -342,194 +371,388 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1">
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
         <v>0.51</v>
       </c>
-      <c r="B1">
+      <c r="C1">
         <v>0.52</v>
       </c>
-      <c r="C1">
+      <c r="D1">
         <v>0.4</v>
       </c>
-      <c r="D1">
+      <c r="E1">
         <v>0.64</v>
       </c>
-      <c r="E1">
+      <c r="F1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="F1">
+      <c r="G1">
         <v>0.6</v>
       </c>
-      <c r="G1">
+      <c r="H1">
         <v>0.85</v>
       </c>
-      <c r="H1">
+      <c r="I1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I1">
+      <c r="J1">
         <v>0.57999999999999996</v>
       </c>
-      <c r="J1">
+      <c r="K1">
         <v>0.52</v>
       </c>
-      <c r="K1">
+      <c r="L1">
         <v>0.72</v>
       </c>
-      <c r="L1">
+      <c r="M1">
         <v>0.77</v>
       </c>
-      <c r="M1">
+      <c r="N1">
         <v>1.28</v>
       </c>
-      <c r="N1">
+      <c r="O1">
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>0.51</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>0.53</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>0.72</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.24</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>0.44</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.69</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>0.76</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.44</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.31</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0.44</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.85</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0.93</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>1.25</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>0.37</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>0.3</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.36</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.27</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.34</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.35</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.23</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.16</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.32</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.37</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.67</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>0.38</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
+    <row r="4" spans="1:15">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>0.34</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>0.15</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>0.34</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.26</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>0.35</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.42</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.37</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.26</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>0.32</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.38</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>0.35</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>0.42</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>0.3</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C5">
+        <v>0.26</v>
+      </c>
+      <c r="D5">
+        <v>0.38</v>
+      </c>
+      <c r="E5">
+        <v>0.38</v>
+      </c>
+      <c r="F5">
+        <v>0.4</v>
+      </c>
+      <c r="G5">
+        <v>0.6</v>
+      </c>
+      <c r="H5">
+        <v>0.48</v>
+      </c>
+      <c r="I5">
+        <v>0.52</v>
+      </c>
+      <c r="J5">
+        <v>0.42</v>
+      </c>
+      <c r="K5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="L5">
+        <v>0.59</v>
+      </c>
+      <c r="M5">
+        <v>0.95</v>
+      </c>
+      <c r="N5">
+        <v>0.98</v>
+      </c>
+      <c r="O5">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>0.39</v>
+      </c>
+      <c r="C6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.36</v>
+      </c>
+      <c r="E6">
+        <v>0.52</v>
+      </c>
+      <c r="F6">
+        <v>0.33</v>
+      </c>
+      <c r="G6">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>0.53</v>
+      </c>
+      <c r="I6">
+        <v>0.45</v>
+      </c>
+      <c r="J6">
+        <v>0.23</v>
+      </c>
+      <c r="K6">
+        <v>0.52</v>
+      </c>
+      <c r="L6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="M6">
+        <v>0.98</v>
+      </c>
+      <c r="N6">
+        <v>1.05</v>
+      </c>
+      <c r="O6">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="C7">
+        <v>0.19</v>
+      </c>
+      <c r="D7">
+        <v>0.39</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7">
+        <v>0.24</v>
+      </c>
+      <c r="G7">
+        <v>0.42</v>
+      </c>
+      <c r="H7">
+        <v>0.2</v>
+      </c>
+      <c r="I7">
+        <v>0.18</v>
+      </c>
+      <c r="J7">
+        <v>0.36</v>
+      </c>
+      <c r="K7">
+        <v>0.3</v>
+      </c>
+      <c r="L7">
+        <v>0.3</v>
+      </c>
+      <c r="M7">
+        <v>0.39</v>
+      </c>
+      <c r="N7">
+        <v>0.4</v>
+      </c>
+      <c r="O7">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.36</v>
+      </c>
+      <c r="C8">
+        <v>0.24</v>
+      </c>
+      <c r="D8">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E8">
+        <v>0.48</v>
+      </c>
+      <c r="F8">
+        <v>0.19</v>
+      </c>
+      <c r="G8">
+        <v>0.32</v>
+      </c>
+      <c r="H8">
+        <v>0.43</v>
+      </c>
+      <c r="I8">
+        <v>0.22</v>
+      </c>
+      <c r="J8">
+        <v>0.5</v>
+      </c>
+      <c r="K8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="L8">
+        <v>0.26</v>
+      </c>
+      <c r="M8">
+        <v>0.3</v>
+      </c>
+      <c r="N8">
+        <v>0.45</v>
+      </c>
+      <c r="O8">
+        <v>0.43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>